<commit_message>
Updated ReadMe and Figures
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Research\Neil McNaughton\Rhys\PsychoPy\StopSignalTask\psychopy_builder_version\V2p0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Research\Neil McNaughton\Rhys\PsychoPy\StopSignalTask\psychopy_builder_version\EEG\V1p1_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4663C9C4-BFD4-4419-9C94-166ACB8631B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FD2660-CA64-4383-8F73-D141C28073BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7245" windowHeight="7980" xr2:uid="{D55FC95E-A168-4840-A5D5-EF12F1130B60}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>practice</t>
   </si>
   <si>
-    <t>fMRI</t>
+    <t>EEG</t>
   </si>
 </sst>
 </file>
@@ -399,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DA7D4A-2E26-4B5B-B55E-7ADBA3EB8D51}">
   <dimension ref="A1:D427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="C296" sqref="C296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>